<commit_message>
Creation de projet avec structure mvc
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -51,6 +51,27 @@
   </si>
   <si>
     <t>Création repo</t>
+  </si>
+  <si>
+    <t>création de la documentation de projet</t>
+  </si>
+  <si>
+    <t>intro, objectif ajouter dans la doc</t>
+  </si>
+  <si>
+    <t>planification initiale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">préparatin des logiciels a utiliser </t>
+  </si>
+  <si>
+    <t>phpStorm, MySQL workbench, HeidiSQL</t>
+  </si>
+  <si>
+    <t>création du projet sur phpStorm</t>
+  </si>
+  <si>
+    <t>index &amp; structure MVC</t>
   </si>
 </sst>
 </file>
@@ -58,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,20 +113,20 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="168" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -124,13 +145,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0">
+  <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date " dataDxfId="3"/>
-    <tableColumn id="2" name="Début" dataDxfId="0"/>
+    <tableColumn id="2" name="Début" dataDxfId="2"/>
     <tableColumn id="3" name="Fin" dataDxfId="1"/>
-    <tableColumn id="4" name="Total" dataDxfId="2">
+    <tableColumn id="4" name="Total" dataDxfId="0">
       <calculatedColumnFormula>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Titre"/>
@@ -403,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,9 +505,99 @@
       <c r="B4" s="2">
         <v>0.4375</v>
       </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
       <c r="D4" s="2">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>-0.4375</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44683</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D5" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44683</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="D6" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D7" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update planification initiale & MCD
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -56,18 +56,12 @@
     <t>création de la documentation de projet</t>
   </si>
   <si>
-    <t>intro, objectif ajouter dans la doc</t>
-  </si>
-  <si>
     <t>planification initiale</t>
   </si>
   <si>
     <t xml:space="preserve">préparatin des logiciels a utiliser </t>
   </si>
   <si>
-    <t>phpStorm, MySQL workbench, HeidiSQL</t>
-  </si>
-  <si>
     <t>création du projet sur phpStorm</t>
   </si>
   <si>
@@ -77,7 +71,28 @@
     <t>MCD</t>
   </si>
   <si>
-    <t>création du mcd su draw.io</t>
+    <t>User stories</t>
+  </si>
+  <si>
+    <t>meeting avec chef de projet</t>
+  </si>
+  <si>
+    <t>Création du sprint 1 et ajout des user stories + revue</t>
+  </si>
+  <si>
+    <t>Création des user stories dans ice scrum</t>
+  </si>
+  <si>
+    <t>Création du mcd su draw.io</t>
+  </si>
+  <si>
+    <t>PhpStorm, MySQL workbench, HeidiSQL</t>
+  </si>
+  <si>
+    <t>Intro, objectif ajouter dans la doc</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -124,7 +139,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
@@ -151,17 +169,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Date " dataDxfId="3"/>
-    <tableColumn id="2" name="Début" dataDxfId="2"/>
-    <tableColumn id="3" name="Fin" dataDxfId="1"/>
-    <tableColumn id="4" name="Total" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G11" totalsRowShown="0">
+  <autoFilter ref="A1:G11"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Date " dataDxfId="4"/>
+    <tableColumn id="2" name="Début" dataDxfId="3"/>
+    <tableColumn id="3" name="Fin" dataDxfId="2"/>
+    <tableColumn id="4" name="Total" dataDxfId="1">
       <calculatedColumnFormula>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Titre"/>
     <tableColumn id="6" name="Description"/>
+    <tableColumn id="7" name="Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -430,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +464,7 @@
     <col min="6" max="6" width="74.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +483,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44683</v>
       </c>
@@ -485,8 +507,9 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44683</v>
       </c>
@@ -503,8 +526,9 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44683</v>
       </c>
@@ -522,10 +546,11 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44683</v>
       </c>
@@ -540,10 +565,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44683</v>
       </c>
@@ -558,13 +584,14 @@
         <v>3.1249999999999889E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44684</v>
       </c>
@@ -579,13 +606,14 @@
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44684</v>
       </c>
@@ -600,35 +628,63 @@
         <v>6.944444444444442E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44684</v>
       </c>
+      <c r="B9" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D9" s="2">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44684</v>
       </c>
+      <c r="B10" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.67361111111111116</v>
+      </c>
       <c r="D10" s="2">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="2">
-        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update doc & mcd
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -93,6 +93,33 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Correction planification initiale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction de la planification initiale et livraison périodique </t>
+  </si>
+  <si>
+    <t>Documentation de projet</t>
+  </si>
+  <si>
+    <t>Élaboration de la stratégie de test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous avons revu le MCD afin de le corriger </t>
+  </si>
+  <si>
+    <t>Correction MCD</t>
+  </si>
+  <si>
+    <t>J'ai corriger le mcd. J'ai ajouter la date d'anniversaire dans la table user j'ai supprimer les colone targetedAreas et Type pour en créer des tables appart entier et j'ai rajouter la colonne matériel</t>
+  </si>
+  <si>
+    <t>Creation des tests d'acceptation sprint 1</t>
+  </si>
+  <si>
+    <t>Creation des Maquettes</t>
   </si>
 </sst>
 </file>
@@ -131,29 +158,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,18 +231,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G11" totalsRowShown="0">
-  <autoFilter ref="A1:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G35" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:G35"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Date " dataDxfId="4"/>
-    <tableColumn id="2" name="Début" dataDxfId="3"/>
-    <tableColumn id="3" name="Fin" dataDxfId="2"/>
-    <tableColumn id="4" name="Total" dataDxfId="1">
+    <tableColumn id="1" name="Date " dataDxfId="8"/>
+    <tableColumn id="2" name="Début" dataDxfId="7"/>
+    <tableColumn id="3" name="Fin" dataDxfId="6"/>
+    <tableColumn id="4" name="Total" dataDxfId="5">
       <calculatedColumnFormula>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Titre"/>
-    <tableColumn id="6" name="Description"/>
-    <tableColumn id="7" name="Type" dataDxfId="0"/>
+    <tableColumn id="5" name="Titre" dataDxfId="4"/>
+    <tableColumn id="6" name="Description" dataDxfId="3"/>
+    <tableColumn id="7" name="Type" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -449,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,226 +527,577 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="6">
         <v>44683</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="7">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="6">
         <v>44683</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="7">
         <v>0.4375</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="6">
         <v>44683</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>0.4375</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="7">
         <v>0.5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="6">
         <v>44683</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="7">
         <v>0.5625</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="7">
         <v>0.625</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="6">
         <v>44683</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>0.67013888888888884</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>3.1249999999999889E-2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="6">
         <v>44684</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="7">
         <v>0.375</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="6">
         <v>44684</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="7">
         <v>0.375</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>6.944444444444442E-2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="6">
         <v>44684</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="7">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>6.597222222222221E-2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="6">
         <v>44684</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="7">
         <v>0.67361111111111116</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="2">
-        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="A11" s="6">
+        <v>44684</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D11" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D12" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D13" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D14" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D15" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D16" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create mockups % update mcd add programs table
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Creation des Maquettes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création Maquettes </t>
+  </si>
+  <si>
+    <t>Création Main Page, SignUp Page et Create Program</t>
+  </si>
+  <si>
+    <t>Création Personal Programs, Personal Program, Exercice details, Create exercise</t>
+  </si>
+  <si>
+    <t>J'ai du ajouter une table "programs" pour les programmes des utilisateurs</t>
   </si>
 </sst>
 </file>
@@ -186,12 +198,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -217,6 +223,12 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -231,18 +243,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G35" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G35"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Date " dataDxfId="8"/>
-    <tableColumn id="2" name="Début" dataDxfId="7"/>
-    <tableColumn id="3" name="Fin" dataDxfId="6"/>
-    <tableColumn id="4" name="Total" dataDxfId="5">
+    <tableColumn id="1" name="Date " dataDxfId="6"/>
+    <tableColumn id="2" name="Début" dataDxfId="5"/>
+    <tableColumn id="3" name="Fin" dataDxfId="4"/>
+    <tableColumn id="4" name="Total" dataDxfId="3">
       <calculatedColumnFormula>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Titre" dataDxfId="4"/>
-    <tableColumn id="6" name="Description" dataDxfId="3"/>
-    <tableColumn id="7" name="Type" dataDxfId="2"/>
+    <tableColumn id="5" name="Titre" dataDxfId="2"/>
+    <tableColumn id="6" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" name="Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -514,7 +526,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,31 +880,53 @@
       <c r="E16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D17" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D18" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update mcd & create use case
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>J'ai du ajouter une table "programs" pour les programmes des utilisateurs</t>
+  </si>
+  <si>
+    <t>Discussion avec chef de projet</t>
+  </si>
+  <si>
+    <t>Le MCD n'étais pas encore au points do</t>
+  </si>
+  <si>
+    <t>Ajout des maquettes et modification de la stratégie de tests</t>
+  </si>
+  <si>
+    <t>Correction du MCD</t>
   </si>
 </sst>
 </file>
@@ -526,7 +538,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,55 +942,91 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.6875</v>
+      </c>
       <c r="D19" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="6">
+        <v>44686</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.6875</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D20" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="6">
+        <v>44687</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.375</v>
+      </c>
       <c r="D21" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="8"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="6">
+        <v>44687</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D22" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6">
+        <v>44687</v>
+      </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7">
@@ -990,7 +1038,9 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="6">
+        <v>44687</v>
+      </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7">

</xml_diff>

<commit_message>
admin page created add places programs and areas
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -229,6 +229,51 @@
   </si>
   <si>
     <t>j'ai telecharger le template sur mon projet</t>
+  </si>
+  <si>
+    <t>implemenation du template pour gabarit</t>
+  </si>
+  <si>
+    <t>implemantation de la page d'acceuil</t>
+  </si>
+  <si>
+    <t>implemantation de la page de login</t>
+  </si>
+  <si>
+    <t>implementation de la page de signup</t>
+  </si>
+  <si>
+    <t>avec un peut d'aide de samuel mon collègue de classe</t>
+  </si>
+  <si>
+    <t>implementation de la fonction login</t>
+  </si>
+  <si>
+    <t>implementation de la fonction signup</t>
+  </si>
+  <si>
+    <t>j'ai développer une partie de la fonction de signup (récuperer les info, hash password )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai créer les fonction pour ajouter un item dans la base de donnée </t>
+  </si>
+  <si>
+    <t>création de la fonction tryLogin qui a pour but de se connecter</t>
+  </si>
+  <si>
+    <t>implementation des helpers</t>
+  </si>
+  <si>
+    <t>dev la fonction helpers qui modifie les boutons de connexion en bouton de deconnexion et de page personnel</t>
+  </si>
+  <si>
+    <t>dev de la fonction de flashmessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correction bug affichage </t>
+  </si>
+  <si>
+    <t>quand je me connecte ca affichais la page d'acceuil et la page de sign up le problème était un break dans l'index</t>
   </si>
 </sst>
 </file>
@@ -340,8 +385,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G42" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:G57" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G57"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Date " dataDxfId="6"/>
     <tableColumn id="2" name="Début" dataDxfId="5"/>
@@ -623,10 +668,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,88 +1496,364 @@
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="6">
+        <v>44691</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="D36" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="6">
+        <v>44691</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.44097222222222227</v>
+      </c>
       <c r="D37" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="8"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="F37" s="8"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="A38" s="6">
+        <v>44691</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="D38" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="8"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="F38" s="8"/>
       <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
+      <c r="A39" s="6">
+        <v>44691</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D39" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="8"/>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="F39" s="8"/>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>44691</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D40" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+      <c r="A41" s="6">
+        <v>44691</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D41" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+        <v>3.4722222222222321E-2</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="6">
+        <v>44692</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D42" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>44692</v>
+      </c>
+      <c r="B43" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D43" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>44692</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D44" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44692</v>
+      </c>
+      <c r="B45" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C45" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D45" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>44692</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7">
+        <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
+        <v>0</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1828,7 +2149,7 @@
       </c>
       <c r="E24" s="2">
         <f>SUM(B:B)</f>
-        <v>1.2395833333333321</v>
+        <v>1.5972222222222214</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,7 +2259,7 @@
       </c>
       <c r="B35" s="2">
         <f>Feuil1!D36</f>
-        <v>0</v>
+        <v>6.5972222222222265E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1948,7 +2269,7 @@
       </c>
       <c r="B36" s="2">
         <f>Feuil1!D37</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,7 +2279,7 @@
       </c>
       <c r="B37" s="2">
         <f>Feuil1!D38</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1968,7 +2289,7 @@
       </c>
       <c r="B38" s="2">
         <f>Feuil1!D39</f>
-        <v>0</v>
+        <v>3.1249999999999944E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1978,7 +2299,7 @@
       </c>
       <c r="B39" s="2">
         <f>Feuil1!D40</f>
-        <v>0</v>
+        <v>3.1249999999999889E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1988,7 +2309,7 @@
       </c>
       <c r="B40" s="2">
         <f>Feuil1!D41</f>
-        <v>0</v>
+        <v>3.4722222222222321E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1998,7 +2319,7 @@
       </c>
       <c r="B41" s="2">
         <f>Feuil1!D42</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2329,7 @@
       </c>
       <c r="B42" s="2">
         <f>Feuil1!D43</f>
-        <v>0</v>
+        <v>4.8611111111111049E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2018,7 +2339,7 @@
       </c>
       <c r="B43" s="2">
         <f>Feuil1!D44</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2028,7 +2349,7 @@
       </c>
       <c r="B44" s="2">
         <f>Feuil1!D45</f>
-        <v>0</v>
+        <v>3.1249999999999944E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add a place program and targeted areas created plus delete elements
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -274,6 +274,60 @@
   </si>
   <si>
     <t>quand je me connecte ca affichais la page d'acceuil et la page de sign up le problème était un break dans l'index</t>
+  </si>
+  <si>
+    <t>Implementation page Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai créer la page admin et j'y ai ajouter les fromulaires pour ajouter </t>
+  </si>
+  <si>
+    <t>fonction ajouter pour places</t>
+  </si>
+  <si>
+    <t>j'ai créer les fonction pour pouvoir ajouter un lieu dans la bdd</t>
+  </si>
+  <si>
+    <t>fonction ajouter pour programmes et zones ciblé</t>
+  </si>
+  <si>
+    <t>j'ai créer les fonction pour ajouter un programme et une zone ciblée dans la bdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage deselement créer </t>
+  </si>
+  <si>
+    <t>j'ai implementer l'affichage des elements puis j'ai réflechis a comment les supprimer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">création de la fonction pour supprimer </t>
+  </si>
+  <si>
+    <t>j'ai créer la fonction pour supprimer un lieu de la bdd</t>
+  </si>
+  <si>
+    <t>un flashmessage apparait indiquant soit que le champ est vide soit que le lieu a déjà été créer</t>
+  </si>
+  <si>
+    <t>gestion des exceptions pour la création de donnée pour lieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestion des exceptions pour la création de donnée pour programmes et zones </t>
+  </si>
+  <si>
+    <t>création de la page Creation d'exercice</t>
+  </si>
+  <si>
+    <t>implementation du formulaire pour créer un ex</t>
+  </si>
+  <si>
+    <t>revue du mld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai remarquer que ma base de donnée n'etais pas correcte je dois retirer le la difficulter et le matériel de la table exercice pour en créer deux nouvelles tables </t>
+  </si>
+  <si>
+    <t>préparation et rendu périodique</t>
   </si>
 </sst>
 </file>
@@ -670,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1437,9 @@
       <c r="F30" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="7"/>
+      <c r="G30" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
@@ -1405,7 +1461,9 @@
       <c r="F31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="7"/>
+      <c r="G31" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
@@ -1427,7 +1485,9 @@
       <c r="F32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
@@ -1449,7 +1509,9 @@
       <c r="F33" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -1459,11 +1521,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="C34" s="7">
-        <v>0.62847222222222221</v>
+        <v>0.64930555555555558</v>
       </c>
       <c r="D34" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>2.430555555555558E-2</v>
+        <v>4.5138888888888951E-2</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>63</v>
@@ -1471,21 +1533,23 @@
       <c r="F34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="7"/>
+      <c r="G34" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>44690</v>
       </c>
       <c r="B35" s="7">
-        <v>0.63888888888888895</v>
+        <v>0.64930555555555558</v>
       </c>
       <c r="C35" s="7">
         <v>0.67013888888888884</v>
       </c>
       <c r="D35" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>3.1249999999999889E-2</v>
+        <v>2.0833333333333259E-2</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>65</v>
@@ -1493,7 +1557,9 @@
       <c r="F35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="7"/>
+      <c r="G35" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
@@ -1515,7 +1581,9 @@
       <c r="F36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="7"/>
+      <c r="G36" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
@@ -1535,7 +1603,9 @@
         <v>68</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="7"/>
+      <c r="G37" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
@@ -1555,7 +1625,9 @@
         <v>69</v>
       </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
@@ -1575,7 +1647,9 @@
         <v>70</v>
       </c>
       <c r="F39" s="8"/>
-      <c r="G39" s="7"/>
+      <c r="G39" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
@@ -1597,7 +1671,9 @@
       <c r="F40" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
@@ -1619,11 +1695,13 @@
       <c r="F41" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>44692</v>
+        <v>44693</v>
       </c>
       <c r="B42" s="7">
         <v>0.36458333333333331</v>
@@ -1641,11 +1719,13 @@
       <c r="F42" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="7"/>
+      <c r="G42" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
-        <v>44692</v>
+        <v>44693</v>
       </c>
       <c r="B43" s="7">
         <v>0.40972222222222227</v>
@@ -1663,11 +1743,13 @@
       <c r="F43" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <v>44692</v>
+        <v>44693</v>
       </c>
       <c r="B44" s="7">
         <v>0.45833333333333331</v>
@@ -1685,11 +1767,13 @@
       <c r="F44" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G44" s="7"/>
+      <c r="G44" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <v>44692</v>
+        <v>44693</v>
       </c>
       <c r="B45" s="7">
         <v>0.47916666666666669</v>
@@ -1707,132 +1791,248 @@
       <c r="F45" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="7"/>
+      <c r="G45" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
-        <v>44692</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+        <v>44693</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.59375</v>
+      </c>
       <c r="D46" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="7"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
+      <c r="A47" s="6">
+        <v>44693</v>
+      </c>
+      <c r="B47" s="7">
+        <v>0.59375</v>
+      </c>
+      <c r="C47" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D47" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>44693</v>
+      </c>
+      <c r="B48" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D48" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>44693</v>
+      </c>
+      <c r="B49" s="7">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D49" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="7"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="A50" s="6">
+        <v>44694</v>
+      </c>
+      <c r="B50" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="D50" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>44694</v>
+      </c>
+      <c r="B51" s="7">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="D51" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>44694</v>
+      </c>
+      <c r="B52" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D52" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="8"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F52" s="8"/>
-      <c r="G52" s="7"/>
+      <c r="G52" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
+      <c r="A53" s="6">
+        <v>44694</v>
+      </c>
+      <c r="B53" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.59375</v>
+      </c>
       <c r="D53" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>44694</v>
+      </c>
+      <c r="B54" s="7">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0.61805555555555558</v>
+      </c>
       <c r="D54" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="7"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
+      <c r="A55" s="6">
+        <v>44694</v>
+      </c>
+      <c r="B55" s="7">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D55" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="8"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="F55" s="8"/>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
+      <c r="A56" s="6">
+        <v>44694</v>
+      </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7">
@@ -1894,7 +2094,7 @@
       </c>
       <c r="E1" s="2">
         <f ca="1">SUMIF(A1:B150,D1,B1:B149)</f>
-        <v>0.78124999999999989</v>
+        <v>0.86458333333333315</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1928,7 +2128,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E4" ca="1" si="0">SUMIF(A3:B152,D3,B3:B151)</f>
-        <v>2.7777777777777735E-2</v>
+        <v>0.80902777777777757</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2149,7 +2349,7 @@
       </c>
       <c r="E24" s="2">
         <f>SUM(B:B)</f>
-        <v>1.5972222222222214</v>
+        <v>1.9756944444444433</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2193,9 +2393,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" t="str">
         <f>Feuil1!G30</f>
-        <v>0</v>
+        <v>Analyze</v>
       </c>
       <c r="B29" s="2">
         <f>Feuil1!D30</f>
@@ -2203,9 +2403,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" t="str">
         <f>Feuil1!G31</f>
-        <v>0</v>
+        <v>Analyze</v>
       </c>
       <c r="B30" s="2">
         <f>Feuil1!D31</f>
@@ -2213,9 +2413,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" t="str">
         <f>Feuil1!G32</f>
-        <v>0</v>
+        <v>Analyze</v>
       </c>
       <c r="B31" s="2">
         <f>Feuil1!D32</f>
@@ -2223,9 +2423,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" t="str">
         <f>Feuil1!G33</f>
-        <v>0</v>
+        <v xml:space="preserve">Documentation </v>
       </c>
       <c r="B32" s="2">
         <f>Feuil1!D33</f>
@@ -2233,29 +2433,29 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" t="str">
         <f>Feuil1!G34</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B33" s="2">
         <f>Feuil1!D34</f>
-        <v>2.430555555555558E-2</v>
+        <v>4.5138888888888951E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" t="str">
         <f>Feuil1!G35</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B34" s="2">
         <f>Feuil1!D35</f>
-        <v>3.1249999999999889E-2</v>
+        <v>2.0833333333333259E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" t="str">
         <f>Feuil1!G36</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B35" s="2">
         <f>Feuil1!D36</f>
@@ -2263,9 +2463,9 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" t="str">
         <f>Feuil1!G37</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B36" s="2">
         <f>Feuil1!D37</f>
@@ -2273,9 +2473,9 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" t="str">
         <f>Feuil1!G38</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B37" s="2">
         <f>Feuil1!D38</f>
@@ -2283,9 +2483,9 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" t="str">
         <f>Feuil1!G39</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B38" s="2">
         <f>Feuil1!D39</f>
@@ -2293,9 +2493,9 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" t="str">
         <f>Feuil1!G40</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B39" s="2">
         <f>Feuil1!D40</f>
@@ -2303,9 +2503,9 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" t="str">
         <f>Feuil1!G41</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B40" s="2">
         <f>Feuil1!D41</f>
@@ -2313,9 +2513,9 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" t="str">
         <f>Feuil1!G42</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B41" s="2">
         <f>Feuil1!D42</f>
@@ -2323,9 +2523,9 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" t="str">
         <f>Feuil1!G43</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B42" s="2">
         <f>Feuil1!D43</f>
@@ -2333,9 +2533,9 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" t="str">
         <f>Feuil1!G44</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B43" s="2">
         <f>Feuil1!D44</f>
@@ -2343,9 +2543,9 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" t="str">
         <f>Feuil1!G45</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B44" s="2">
         <f>Feuil1!D45</f>
@@ -2353,93 +2553,93 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" t="str">
         <f>Feuil1!G46</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B45" s="2">
         <f>Feuil1!D46</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" t="str">
         <f>Feuil1!G47</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B46" s="2">
         <f>Feuil1!D47</f>
-        <v>0</v>
+        <v>3.472222222222221E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" t="str">
         <f>Feuil1!G48</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B47" s="2">
         <f>Feuil1!D48</f>
-        <v>0</v>
+        <v>3.1249999999999889E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" t="str">
         <f>Feuil1!G49</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B48" s="2">
         <f>Feuil1!D49</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" t="str">
         <f>Feuil1!G50</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B49" s="2">
         <f>Feuil1!D50</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" t="str">
         <f>Feuil1!G51</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B50" s="2">
         <f>Feuil1!D51</f>
-        <v>0</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" t="str">
         <f>Feuil1!G52</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B51" s="2">
         <f>Feuil1!D52</f>
-        <v>0</v>
+        <v>5.2083333333333315E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" t="str">
         <f>Feuil1!G53</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B52" s="2">
         <f>Feuil1!D53</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" t="str">
         <f>Feuil1!G54</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B53" s="2">
         <f>Feuil1!D54</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2449,7 +2649,7 @@
       </c>
       <c r="B54" s="2">
         <f>Feuil1!D55</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
doc and del template
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="121">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -334,6 +334,63 @@
   </si>
   <si>
     <t>Avec le chef de projet on est passé a travèrs les differentes users stories. Il me faut finir la partie de création d'ex de la partie admin, modifier le mcd mld et la base de donné en créeant une nouvelle table materials ainsi que créer des messages d'erreur pour les inputs vide dans le sign in et login</t>
+  </si>
+  <si>
+    <t>modification mcd mld bdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai modifier le mcd et mld puis la base de donnée en créeant une nouvelle table materials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">affichage des messages d'erreures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai ajouter des messages d'erreures pour les login et sign in. Si les inputs sont vide si l'email existe déjà </t>
+  </si>
+  <si>
+    <t>fontion ajout supprimer materiel</t>
+  </si>
+  <si>
+    <t>j'ai ajouter la possibilité de créer du nouveau matériel et de le supprimmer</t>
+  </si>
+  <si>
+    <t>ajout des exeption pour matériel</t>
+  </si>
+  <si>
+    <t>des messages d'erreures s'affichent maintent quand on veut créer un matériel : redondance champs vide</t>
+  </si>
+  <si>
+    <t>implementation des inputs pour créer un exercice</t>
+  </si>
+  <si>
+    <t>j'ai rajouter les inputs nessessaire pour l'upload d'un exercice</t>
+  </si>
+  <si>
+    <t>la fonction dans le modèle n'ajoute pas l'image pour l'instant et n'update pas les table intermediare ex exercise_practice_place</t>
+  </si>
+  <si>
+    <t>création de la fonction permettant de créer un exercice</t>
+  </si>
+  <si>
+    <t>recherche pour upload une image dans le dossier images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dans w3 school j'ai trouver comment upload une image </t>
+  </si>
+  <si>
+    <t>implementation de la fonction d'upload d'image</t>
+  </si>
+  <si>
+    <t>en me basant sur la fonction de w3school j'ai adpter la fonction a mon code puis ai ajouter le nom de l'image dans la fonction pour créer un ex</t>
+  </si>
+  <si>
+    <t>implementation des message d'erreur</t>
+  </si>
+  <si>
+    <t>j'ai implementer les messages d'erreurs pour ( fichier n'est pas une image, fichier trop lourd, fichier déjà existant)</t>
+  </si>
+  <si>
+    <t>ajout de la structure de code dans la doc avec description</t>
   </si>
 </sst>
 </file>
@@ -730,8 +787,8 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2090,9 @@
         <v>99</v>
       </c>
       <c r="F55" s="8"/>
-      <c r="G55" s="7"/>
+      <c r="G55" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
@@ -2053,7 +2112,9 @@
         <v>100</v>
       </c>
       <c r="F56" s="8"/>
-      <c r="G56" s="7"/>
+      <c r="G56" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
@@ -2075,127 +2136,247 @@
       <c r="F57" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
+      <c r="G57" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>44697</v>
+      </c>
+      <c r="B58" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0.44097222222222227</v>
+      </c>
       <c r="D58" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="7"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>44697</v>
+      </c>
+      <c r="B59" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D59" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="7"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="A60" s="6">
+        <v>44697</v>
+      </c>
+      <c r="B60" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.625</v>
+      </c>
       <c r="D60" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>44697</v>
+      </c>
+      <c r="B61" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D61" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>44698</v>
+      </c>
+      <c r="B62" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="D62" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>44698</v>
+      </c>
+      <c r="B63" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D63" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>44698</v>
+      </c>
+      <c r="B64" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0.4375</v>
+      </c>
       <c r="D64" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>44698</v>
+      </c>
+      <c r="B65" s="7">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D65" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
+        <v>6.9444444444444364E-2</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>44698</v>
+      </c>
+      <c r="B66" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D66" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>44698</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D67" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E67" s="8"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="F67" s="8"/>
-      <c r="G67" s="7"/>
+      <c r="G67" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
@@ -2488,7 +2669,7 @@
       </c>
       <c r="E1" s="2">
         <f ca="1">SUMIF(A1:B150,D1,B1:B149)</f>
-        <v>0.86458333333333315</v>
+        <v>0.92708333333333315</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2522,7 +2703,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E4" ca="1" si="0">SUMIF(A3:B152,D3,B3:B151)</f>
-        <v>0.80902777777777757</v>
+        <v>1.1909722222222214</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2743,7 +2924,7 @@
       </c>
       <c r="E24" s="2">
         <f>SUM(B:B)</f>
-        <v>2.0381944444444433</v>
+        <v>2.4513888888888875</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,9 +3218,9 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" t="str">
         <f>Feuil1!G55</f>
-        <v>0</v>
+        <v xml:space="preserve">Documentation </v>
       </c>
       <c r="B54" s="2">
         <f>Feuil1!D55</f>
@@ -3047,9 +3228,9 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" t="str">
         <f>Feuil1!G56</f>
-        <v>0</v>
+        <v>Analyze</v>
       </c>
       <c r="B55" s="2">
         <f>Feuil1!D56</f>
@@ -3057,9 +3238,9 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" t="str">
         <f>Feuil1!G57</f>
-        <v>0</v>
+        <v>Analyze</v>
       </c>
       <c r="B56" s="2">
         <f>Feuil1!D57</f>
@@ -3067,103 +3248,103 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" t="str">
         <f>Feuil1!G58</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B57" s="2">
         <f>Feuil1!D58</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" t="str">
         <f>Feuil1!G59</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B58" s="2">
         <f>Feuil1!D59</f>
-        <v>0</v>
+        <v>6.597222222222221E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" t="str">
         <f>Feuil1!G60</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B59" s="2">
         <f>Feuil1!D60</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" t="str">
         <f>Feuil1!G61</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B60" s="2">
         <f>Feuil1!D61</f>
-        <v>0</v>
+        <v>3.1249999999999889E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" t="str">
         <f>Feuil1!G62</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B61" s="2">
         <f>Feuil1!D62</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" t="str">
         <f>Feuil1!G63</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B62" s="2">
         <f>Feuil1!D63</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" t="str">
         <f>Feuil1!G64</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B63" s="2">
         <f>Feuil1!D64</f>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" t="str">
         <f>Feuil1!G65</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B64" s="2">
         <f>Feuil1!D65</f>
-        <v>0</v>
+        <v>6.9444444444444364E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" t="str">
         <f>Feuil1!G66</f>
-        <v>0</v>
+        <v>Implementation</v>
       </c>
       <c r="B65" s="2">
         <f>Feuil1!D66</f>
-        <v>0</v>
+        <v>3.1249999999999889E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" t="str">
         <f>Feuil1!G67</f>
-        <v>0</v>
+        <v xml:space="preserve">Documentation </v>
       </c>
       <c r="B66" s="2">
         <f>Feuil1!D67</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
create data and create part of program creation program
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="141">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -430,14 +430,36 @@
   </si>
   <si>
     <t xml:space="preserve">ajout du chemin des scripts </t>
+  </si>
+  <si>
+    <t>implementation de la page perso user</t>
+  </si>
+  <si>
+    <t>le user peut aller sur ca page perso on voit les deux dropdown place et program ainsi que le bouton pour créer le programme perso</t>
+  </si>
+  <si>
+    <t>ajout de donnée ex pour créer les programmes</t>
+  </si>
+  <si>
+    <t>reflection pour la logique de création de programme</t>
+  </si>
+  <si>
+    <t>début de la fonction pour créer le programme</t>
+  </si>
+  <si>
+    <t>je peux var_dump les id des exercise qui partagent le meme lieu et programme</t>
+  </si>
+  <si>
+    <t>preparation rendu périodique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -468,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -490,18 +512,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -511,6 +527,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -546,13 +569,13 @@
   <tableColumns count="7">
     <tableColumn id="1" name="Date " dataDxfId="6"/>
     <tableColumn id="2" name="Début" dataDxfId="5"/>
-    <tableColumn id="3" name="Fin" dataDxfId="4"/>
-    <tableColumn id="4" name="Total" dataDxfId="3">
+    <tableColumn id="3" name="Fin" dataDxfId="1"/>
+    <tableColumn id="4" name="Total" dataDxfId="2">
       <calculatedColumnFormula>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Titre" dataDxfId="2"/>
-    <tableColumn id="6" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" name="Type" dataDxfId="0"/>
+    <tableColumn id="5" name="Titre" dataDxfId="0"/>
+    <tableColumn id="6" name="Description" dataDxfId="4"/>
+    <tableColumn id="7" name="Type" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,10 +847,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +863,7 @@
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -862,8 +885,9 @@
       <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44683</v>
       </c>
@@ -887,7 +911,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44683</v>
       </c>
@@ -909,7 +933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44683</v>
       </c>
@@ -933,7 +957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>44683</v>
       </c>
@@ -955,7 +979,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44683</v>
       </c>
@@ -978,8 +1002,9 @@
       <c r="G6" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44684</v>
       </c>
@@ -1003,7 +1028,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>44684</v>
       </c>
@@ -1027,7 +1052,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>44684</v>
       </c>
@@ -1051,7 +1076,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>44684</v>
       </c>
@@ -1075,7 +1100,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>44684</v>
       </c>
@@ -1099,7 +1124,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>44686</v>
       </c>
@@ -1123,7 +1148,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>44686</v>
       </c>
@@ -1147,7 +1172,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>44686</v>
       </c>
@@ -1171,7 +1196,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>44686</v>
       </c>
@@ -1193,7 +1218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>44686</v>
       </c>
@@ -2621,63 +2646,107 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>44701</v>
+      </c>
+      <c r="B77" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C77" s="7">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D77" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>44701</v>
+      </c>
+      <c r="B78" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C78" s="7">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="D78" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E78" s="8"/>
+        <v>6.5972222222222154E-2</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="F78" s="8"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>44701</v>
+      </c>
+      <c r="B79" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C79" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D79" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E79" s="8"/>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="F79" s="8"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>44701</v>
+      </c>
+      <c r="B80" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C80" s="7">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D80" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="G80" s="7"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+      <c r="A81" s="6">
+        <v>44701</v>
+      </c>
+      <c r="B81" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D81" s="7">
         <f>Tableau2[[#This Row],[Fin]]-Tableau2[[#This Row],[Début]]</f>
-        <v>0</v>
-      </c>
-      <c r="E81" s="8"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F81" s="8"/>
       <c r="G81" s="7"/>
     </row>
@@ -3059,7 +3128,7 @@
       </c>
       <c r="E24" s="2">
         <f>SUM(B:B)</f>
-        <v>2.6979166666666652</v>
+        <v>2.9236111111111098</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3579,7 +3648,7 @@
       </c>
       <c r="B76" s="2">
         <f>Feuil1!D77</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3589,7 +3658,7 @@
       </c>
       <c r="B77" s="2">
         <f>Feuil1!D78</f>
-        <v>0</v>
+        <v>6.5972222222222154E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -3599,7 +3668,7 @@
       </c>
       <c r="B78" s="2">
         <f>Feuil1!D79</f>
-        <v>0</v>
+        <v>3.1249999999999944E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -3609,7 +3678,7 @@
       </c>
       <c r="B79" s="2">
         <f>Feuil1!D80</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -3619,7 +3688,7 @@
       </c>
       <c r="B80" s="2">
         <f>Feuil1!D81</f>
-        <v>0</v>
+        <v>2.430555555555558E-2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>